<commit_message>
Add capacitor across strobe relay power
</commit_message>
<xml_diff>
--- a/electrical/StrobeController-BOM.xlsx
+++ b/electrical/StrobeController-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DE9B76-56B9-45C9-B6C8-A543FFA504CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74A57ED-C7E7-4438-A0C0-5AE3E8FE4A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Rectifier Diode</t>
   </si>
@@ -157,6 +157,21 @@
   </si>
   <si>
     <t>J3</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>0.47nF; 50v</t>
+  </si>
+  <si>
+    <t>0805B471K500CT</t>
+  </si>
+  <si>
+    <t>0805</t>
   </si>
 </sst>
 </file>
@@ -795,8 +810,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label(s)" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="8"/>
@@ -1110,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,66 +1257,70 @@
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="D5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="H5" s="5">
         <v>1</v>
       </c>
-      <c r="I5" s="6">
-        <v>1.31</v>
+      <c r="I5" s="8">
+        <v>0.1</v>
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="4"/>
       <c r="F6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="H6" s="5">
         <v>1</v>
       </c>
-      <c r="I6" s="8">
-        <v>0.41</v>
+      <c r="I6" s="6">
+        <v>1.31</v>
       </c>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="5" t="s">
-        <v>37</v>
+      <c r="D7" t="s">
+        <v>35</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
@@ -1311,21 +1330,21 @@
       <c r="H7" s="5">
         <v>1</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>24</v>
+      <c r="I7" s="8">
+        <v>0.41</v>
       </c>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
@@ -1341,44 +1360,63 @@
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11">
-        <f>SUM(H2:H7)</f>
-        <v>7</v>
-      </c>
-      <c r="I9" s="12">
-        <f>SUM(I2:I7)</f>
-        <v>3.0500000000000003</v>
-      </c>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11">
+        <f>SUM(H2:H8)</f>
+        <v>8</v>
+      </c>
+      <c r="I10" s="12">
+        <f>SUM(I2:I8)</f>
+        <v>3.1500000000000004</v>
+      </c>
+      <c r="J10" s="11"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -1440,20 +1478,20 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
@@ -1465,30 +1503,30 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
@@ -1559,6 +1597,11 @@
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>